<commit_message>
Updates to make more toolbox-like
</commit_message>
<xml_diff>
--- a/tbx/nowcastingTemplateData/Example1_tracking.xlsx
+++ b/tbx/nowcastingTemplateData/Example1_tracking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E02DA7-0E55-47DE-922E-1DCAA01761C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B2E379-176D-45B4-9B82-C0402FF19FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="20" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="172">
   <si>
     <t>Date</t>
   </si>
@@ -339,9 +339,6 @@
     <t>Group name</t>
   </si>
   <si>
-    <t>Full name 10</t>
-  </si>
-  <si>
     <t>Full name 11</t>
   </si>
   <si>
@@ -569,6 +566,99 @@
   </si>
   <si>
     <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Full name 10</t>
   </si>
   <si>
     <t> </t>
@@ -1611,11 +1701,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0" tint="-4.89516891994995E-2"/>
+        <color theme="0" tint="-4.88906521805475E-2"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.89516891994995E-2"/>
+          <bgColor theme="0" tint="-4.88906521805475E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1741,11 +1831,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0" tint="-4.89516891994995E-2"/>
+        <color theme="0" tint="-4.88906521805475E-2"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-4.89516891994995E-2"/>
+          <bgColor theme="0" tint="-4.88906521805475E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2601,10 +2691,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.56987193301505046</c:v>
+                  <c:v>0.94593492232226339</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.33615761305287017</c:v>
+                  <c:v>1.1696700450167241E-3</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -2681,10 +2771,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.45082735081176761</c:v>
+                  <c:v>0.92556395177594819</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.29537882948201044</c:v>
+                  <c:v>0.32425794719983647</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -2761,10 +2851,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.45405898397042066</c:v>
+                  <c:v>0.63942374820899262</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.44149452664529831</c:v>
+                  <c:v>0.59807329952981025</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -2841,10 +2931,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.5494021819730901</c:v>
+                  <c:v>0.92134737842481385</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.30058984898206098</c:v>
+                  <c:v>-4.3240353800786113E-2</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -2921,10 +3011,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.56853919396714558</c:v>
+                  <c:v>0.6817992691431648</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.50652543969704489</c:v>
+                  <c:v>0.62939931376445468</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -3001,10 +3091,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.34359322860359021</c:v>
+                  <c:v>-8.5098149328051764E-2</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.38502190356968585</c:v>
+                  <c:v>0.39457613451002643</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -4330,10 +4420,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3" formatCode="0.0">
-                  <c:v>0.34359322860359021</c:v>
+                  <c:v>-8.5098149328051764E-2</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0">
-                  <c:v>0.38502190356968585</c:v>
+                  <c:v>0.39457613451002643</c:v>
                 </c:pt>
               </c:numCache>
               <c:extLst/>
@@ -4841,12 +4931,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.41030889303670498</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.42448670855549347</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4901,10 +4985,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-6.6006917974893553E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-6.2299352514690653E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4960,10 +5044,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>11.757222255527484</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4159270272049049</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5019,10 +5103,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-11.611355055086923</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.4629306389169552</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5106,10 +5190,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.49016917550237188</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31518374432875257</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5375,9 +5459,6 @@
               <c:f>Contributions!$G$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group 1</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -5397,40 +5478,40 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Full name 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Full name 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Full name 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Full name 5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Full name 6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Full name 7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Full name 8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Full name 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Full name 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Full name 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Full name 12</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Full name 10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Full name 11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Full name 3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Full name 9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Full name 2</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>Full name target</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Full name 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Full name 6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Full name 1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Full name 7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Full name 4</c:v>
@@ -5444,20 +5525,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="1">
-                  <c:v>-4.7416059107197719E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1.8751857451705434E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-8.0616733334545089E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.864034266449822E-3</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.3586376510142888E-3</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5477,7 +5558,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Group 2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5505,40 +5586,40 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Full name 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Full name 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Full name 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Full name 5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Full name 6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Full name 7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Full name 8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Full name 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Full name 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Full name 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Full name 12</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Full name 10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Full name 11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Full name 3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Full name 9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Full name 2</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>Full name target</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Full name 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Full name 6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Full name 1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Full name 7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Full name 4</c:v>
@@ -5552,14 +5633,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="4">
-                  <c:v>-2.3908042631783605E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.8713913429467106E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.3972212215584534E-2</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>11.741769456232131</c:v>
@@ -5581,9 +5662,6 @@
               <c:f>Contributions!$I$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Group 3</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -5610,40 +5688,40 @@
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>Full name 2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Full name 3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Full name 4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Full name 5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
+                  <c:v>Full name 6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Full name 7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Full name 8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Full name 9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Full name 10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Full name 11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>Full name 12</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Full name 10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Full name 11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Full name 3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Full name 9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Full name 2</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>Full name target</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Full name 8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Full name 6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Full name 1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Full name 7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>Full name 4</c:v>
@@ -5657,17 +5735,17 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>-11.660518915061418</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.795068486684242E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.8462829947134536E-3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.9522508493098787E-2</c:v>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13377,21 +13455,21 @@
   <sheetData>
     <row r="1" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I1" s="123" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J1" s="106"/>
       <c r="K1" s="107"/>
       <c r="L1" s="123" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N1" s="20"/>
       <c r="O1" s="51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P1" s="28"/>
       <c r="Q1" s="20"/>
       <c r="R1" s="51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S1" s="28"/>
     </row>
@@ -13438,22 +13516,22 @@
         <v>40</v>
       </c>
       <c r="V2" s="111" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="111" t="s">
         <v>92</v>
       </c>
-      <c r="W2" s="111" t="s">
+      <c r="X2" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="111" t="s">
+      <c r="Y2" s="111" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="111" t="s">
+      <c r="Z2" s="111" t="s">
         <v>95</v>
       </c>
-      <c r="Z2" s="111" t="s">
+      <c r="AA2" s="111" t="s">
         <v>96</v>
-      </c>
-      <c r="AA2" s="111" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="17.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -13790,12 +13868,12 @@
       </c>
       <c r="N19" s="11"/>
       <c r="O19" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P19" s="28"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S19" s="28"/>
       <c r="U19" s="122" t="str">
@@ -13804,27 +13882,27 @@
       </c>
       <c r="V19" s="107">
         <f>VLOOKUP(V$2,Range!$A$2:$C$22,MATCH($U19,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.56987193301505046</v>
+        <v>0.94593492232226339</v>
       </c>
       <c r="W19" s="107">
         <f>VLOOKUP(W$2,Range!$A$2:$C$22,MATCH($U19,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.45082735081176761</v>
+        <v>0.92556395177594819</v>
       </c>
       <c r="X19" s="107">
         <f>VLOOKUP(X$2,Range!$A$2:$C$22,MATCH($U19,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.45405898397042066</v>
+        <v>0.63942374820899262</v>
       </c>
       <c r="Y19" s="107">
         <f>VLOOKUP(Y$2,Range!$A$2:$C$22,MATCH($U19,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.5494021819730901</v>
+        <v>0.92134737842481385</v>
       </c>
       <c r="Z19" s="107">
         <f>VLOOKUP(Z$2,Range!$A$2:$C$22,MATCH($U19,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.56853919396714558</v>
+        <v>0.6817992691431648</v>
       </c>
       <c r="AA19" s="107">
         <f>VLOOKUP(AA$2,Range!$A$2:$C$22,MATCH($U19,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.34359322860359021</v>
+        <v>-8.5098149328051764E-2</v>
       </c>
     </row>
     <row r="20" spans="1:27" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
@@ -13862,7 +13940,7 @@
       <c r="P20" s="30"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S20" s="30"/>
       <c r="U20" s="122" t="str">
@@ -13871,27 +13949,27 @@
       </c>
       <c r="V20" s="107">
         <f>VLOOKUP(V$2,Range!$A$2:$C$22,MATCH($U20,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.33615761305287017</v>
+        <v>1.1696700450167241E-3</v>
       </c>
       <c r="W20" s="107">
         <f>VLOOKUP(W$2,Range!$A$2:$C$22,MATCH($U20,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.29537882948201044</v>
+        <v>0.32425794719983647</v>
       </c>
       <c r="X20" s="107">
         <f>VLOOKUP(X$2,Range!$A$2:$C$22,MATCH($U20,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.44149452664529831</v>
+        <v>0.59807329952981025</v>
       </c>
       <c r="Y20" s="107">
         <f>VLOOKUP(Y$2,Range!$A$2:$C$22,MATCH($U20,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.30058984898206098</v>
+        <v>-4.3240353800786113E-2</v>
       </c>
       <c r="Z20" s="107">
         <f>VLOOKUP(Z$2,Range!$A$2:$C$22,MATCH($U20,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.50652543969704489</v>
+        <v>0.62939931376445468</v>
       </c>
       <c r="AA20" s="107">
         <f>VLOOKUP(AA$2,Range!$A$2:$C$22,MATCH($U20,Range!$A$1:$C$1,0),FALSE)</f>
-        <v>0.38502190356968585</v>
+        <v>0.39457613451002643</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.4">
@@ -13919,12 +13997,12 @@
     <row r="22" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N22" s="20"/>
       <c r="O22" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P22" s="28"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S22" s="28"/>
     </row>
@@ -14061,12 +14139,12 @@
       <c r="H40" s="121"/>
       <c r="N40" s="11"/>
       <c r="O40" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P40" s="28"/>
       <c r="Q40" s="11"/>
       <c r="R40" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S40" s="28"/>
     </row>
@@ -14080,12 +14158,12 @@
       <c r="H41" s="121"/>
       <c r="N41" s="11"/>
       <c r="O41" s="48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="P41" s="30"/>
       <c r="Q41" s="11"/>
       <c r="R41" s="48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S41" s="30"/>
     </row>
@@ -15006,7 +15084,7 @@
         <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3">
         <v>-0.2956479611200114</v>
@@ -15112,7 +15190,7 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="C4">
         <v>-0.60346473725360561</v>
@@ -15215,7 +15293,7 @@
         <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>-0.41928636444622636</v>
@@ -15318,7 +15396,7 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6">
         <v>1.2105212424580623</v>
@@ -15421,7 +15499,7 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>0.10349424620029879</v>
@@ -15527,7 +15605,7 @@
         <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8">
         <v>8.0146713464143191E-2</v>
@@ -15630,7 +15708,7 @@
         <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9">
         <v>3.6437407062214253E-2</v>
@@ -15733,7 +15811,7 @@
         <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10">
         <v>-0.56123924451140605</v>
@@ -15836,7 +15914,7 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11">
         <v>-0.5636297655136504</v>
@@ -15942,7 +16020,7 @@
         <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <v>-1.1144181479174524</v>
@@ -16045,7 +16123,7 @@
         <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13">
         <v>0.11601606469654289</v>
@@ -16148,7 +16226,7 @@
         <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>-0.15089889861107361</v>
@@ -16251,7 +16329,7 @@
         <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>0.23093034152569594</v>
@@ -16763,7 +16841,7 @@
     </row>
     <row r="23" spans="1:35" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>0.23093034152569594</v>
@@ -17112,101 +17190,101 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2">
-        <v>0.56987193301505046</v>
+        <v>0.94593492232226339</v>
       </c>
       <c r="C2">
-        <v>0.33615761305287017</v>
+        <v>1.1696700450167241E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3">
-        <v>0.45082735081176761</v>
+        <v>0.92556395177594819</v>
       </c>
       <c r="C3">
-        <v>0.29537882948201044</v>
+        <v>0.32425794719983647</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4">
-        <v>0.45405898397042066</v>
+        <v>0.63942374820899262</v>
       </c>
       <c r="C4">
-        <v>0.44149452664529831</v>
+        <v>0.59807329952981025</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5">
-        <v>0.5494021819730901</v>
+        <v>0.92134737842481385</v>
       </c>
       <c r="C5">
-        <v>0.30058984898206098</v>
+        <v>-4.3240353800786113E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6">
-        <v>0.56853919396714558</v>
+        <v>0.6817992691431648</v>
       </c>
       <c r="C6">
-        <v>0.50652543969704489</v>
+        <v>0.62939931376445468</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7">
-        <v>0.34359322860359021</v>
+        <v>-8.5098149328051764E-2</v>
       </c>
       <c r="C7">
-        <v>0.38502190356968585</v>
+        <v>0.39457613451002643</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9">
-        <v>0.34359322860359021</v>
+        <v>-8.5098149328051764E-2</v>
       </c>
       <c r="C9">
-        <v>0.29537882948201044</v>
+        <v>-4.3240353800786113E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10">
-        <v>0.56987193301505046</v>
+        <v>0.94593492232226339</v>
       </c>
       <c r="C10">
-        <v>0.50652543969704489</v>
+        <v>0.62939931376445468</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11">
-        <v>0.49016917550237188</v>
+        <v>0.81504087593124508</v>
       </c>
       <c r="C11">
-        <v>0.31518374432875257</v>
+        <v>1.087879510367447</v>
       </c>
     </row>
   </sheetData>
@@ -17220,7 +17298,7 @@
   <dimension ref="A1:W95"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I22"/>
+      <selection activeCell="G2" sqref="G2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -17262,10 +17340,10 @@
         <v>57</v>
       </c>
       <c r="B2">
-        <v>0.49016917550237188</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.31518374432875257</v>
+        <v>0</v>
       </c>
       <c r="P2" s="18"/>
       <c r="Q2" s="67" t="s">
@@ -17285,10 +17363,10 @@
         <v>58</v>
       </c>
       <c r="B4">
-        <v>-6.6006917974893553E-2</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>-6.2299352514690653E-2</v>
+        <v>0</v>
       </c>
       <c r="P4" s="18"/>
       <c r="Q4" s="19"/>
@@ -17299,10 +17377,10 @@
         <v>59</v>
       </c>
       <c r="B5">
-        <v>11.757222255527484</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>1.4159270272049049</v>
+        <v>0</v>
       </c>
       <c r="P5" s="18"/>
       <c r="Q5" s="19"/>
@@ -17313,10 +17391,10 @@
         <v>60</v>
       </c>
       <c r="B6">
-        <v>-11.611355055086923</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>-1.4629306389169552</v>
+        <v>0</v>
       </c>
       <c r="P6" s="18"/>
       <c r="Q6" s="19"/>
@@ -17326,42 +17404,54 @@
       <c r="A7" t="s">
         <v>61</v>
       </c>
-      <c r="B7">
-        <v>0.41030889303670498</v>
-      </c>
-      <c r="C7">
-        <v>0.42448670855549347</v>
+      <c r="G7" t="s">
+        <v>90</v>
       </c>
       <c r="P7" s="18"/>
       <c r="Q7" s="19"/>
       <c r="R7" s="18"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
       </c>
       <c r="P8" s="18"/>
       <c r="Q8" s="19"/>
       <c r="R8" s="18"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" t="s">
-        <v>60</v>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="P9" s="18"/>
       <c r="Q9" s="19"/>
@@ -17369,28 +17459,28 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A10" s="53" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B10" s="53">
-        <v>-11.660518915061418</v>
+        <v>0</v>
       </c>
       <c r="C10" s="53">
-        <v>-1.4283023974407905</v>
+        <v>0</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E10" s="53">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" s="53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53">
-        <v>-11.660518915061418</v>
-      </c>
+      <c r="H10" s="53">
+        <v>0</v>
+      </c>
+      <c r="I10" s="53"/>
       <c r="J10" s="53"/>
       <c r="P10" s="18"/>
       <c r="Q10" s="19"/>
@@ -17398,27 +17488,27 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A11" s="105" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" s="53">
-        <v>-4.7416059107197719E-2</v>
+        <v>0</v>
       </c>
       <c r="C11" s="53">
-        <v>-3.8600598628376316E-2</v>
+        <v>0</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E11" s="53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="53">
-        <v>-4.7416059107197719E-2</v>
-      </c>
-      <c r="H11" s="53"/>
+        <v>59</v>
+      </c>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53">
+        <v>0</v>
+      </c>
       <c r="I11" s="53"/>
       <c r="J11" s="53"/>
       <c r="P11" s="18"/>
@@ -17427,27 +17517,27 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A12" s="53" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B12" s="53">
-        <v>-1.8751857451705434E-2</v>
+        <v>0</v>
       </c>
       <c r="C12" s="53">
-        <v>-1.9039098132844205E-2</v>
+        <v>0</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E12" s="53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="53">
-        <v>-1.8751857451705434E-2</v>
-      </c>
-      <c r="H12" s="53"/>
+        <v>59</v>
+      </c>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53">
+        <v>0</v>
+      </c>
       <c r="I12" s="53"/>
       <c r="J12" s="53"/>
       <c r="P12" s="18"/>
@@ -17456,28 +17546,28 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A13" s="53" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B13" s="53">
-        <v>-8.0616733334545089E-3</v>
+        <v>0</v>
       </c>
       <c r="C13" s="53">
-        <v>-9.1775578679579219E-3</v>
+        <v>0</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="E13" s="53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="53">
-        <v>-8.0616733334545089E-3</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G13" s="53"/>
       <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
+      <c r="I13" s="53">
+        <v>0</v>
+      </c>
       <c r="J13" s="53"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="19"/>
@@ -17485,28 +17575,28 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A14" s="53" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B14" s="53">
-        <v>-2.3908042631783605E-3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="53">
-        <v>-2.059435115409056E-2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E14" s="53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G14" s="53"/>
-      <c r="H14" s="53">
-        <v>-2.3908042631783605E-3</v>
-      </c>
-      <c r="I14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53">
+        <v>0</v>
+      </c>
       <c r="J14" s="53"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="19"/>
@@ -17514,28 +17604,28 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A15" s="53" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B15" s="53">
-        <v>3.864034266449822E-3</v>
+        <v>0</v>
       </c>
       <c r="C15" s="53">
-        <v>-6.4304518172460454E-3</v>
+        <v>0</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E15" s="53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="53">
-        <v>3.864034266449822E-3</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G15" s="53"/>
       <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
+      <c r="I15" s="53">
+        <v>0</v>
+      </c>
       <c r="J15" s="53"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="19"/>
@@ -17543,28 +17633,28 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A16" s="53" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B16" s="53">
-        <v>3.8713913429467106E-3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="53">
-        <v>-1.1394420805211209E-2</v>
+        <v>0</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E16" s="53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="53" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G16" s="53"/>
-      <c r="H16" s="53">
-        <v>3.8713913429467106E-3</v>
-      </c>
-      <c r="I16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53">
+        <v>0</v>
+      </c>
       <c r="J16" s="53"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="19"/>
@@ -17572,16 +17662,16 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A17" s="53" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B17" s="53">
-        <v>4.3586376510142888E-3</v>
+        <v>0</v>
       </c>
       <c r="C17" s="53">
-        <v>1.0948353931733839E-2</v>
+        <v>0</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E17" s="53">
         <v>1</v>
@@ -17590,7 +17680,7 @@
         <v>58</v>
       </c>
       <c r="G17" s="53">
-        <v>4.3586376510142888E-3</v>
+        <v>0</v>
       </c>
       <c r="H17" s="53"/>
       <c r="I17" s="53"/>
@@ -17601,28 +17691,28 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" s="53" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B18" s="53">
-        <v>9.795068486684242E-3</v>
+        <v>0</v>
       </c>
       <c r="C18" s="53">
-        <v>-3.1654515898683393E-2</v>
+        <v>0</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="E18" s="53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G18" s="53"/>
+        <v>58</v>
+      </c>
+      <c r="G18" s="53">
+        <v>0</v>
+      </c>
       <c r="H18" s="53"/>
-      <c r="I18" s="53">
-        <v>9.795068486684242E-3</v>
-      </c>
+      <c r="I18" s="53"/>
       <c r="J18" s="53"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="19"/>
@@ -17630,28 +17720,28 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A19" s="105" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B19" s="53">
-        <v>9.8462829947134536E-3</v>
+        <v>0</v>
       </c>
       <c r="C19" s="53">
-        <v>3.5645742591182616E-3</v>
+        <v>0</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E19" s="53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="53"/>
+        <v>58</v>
+      </c>
+      <c r="G19" s="53">
+        <v>0</v>
+      </c>
       <c r="H19" s="53"/>
-      <c r="I19" s="53">
-        <v>9.8462829947134536E-3</v>
-      </c>
+      <c r="I19" s="53"/>
       <c r="J19" s="53"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="19"/>
@@ -17659,27 +17749,27 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" s="53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B20" s="53">
-        <v>1.3972212215584534E-2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="53">
-        <v>9.955863245362037E-5</v>
+        <v>0</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E20" s="53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53">
-        <v>1.3972212215584534E-2</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G20" s="53">
+        <v>0</v>
+      </c>
+      <c r="H20" s="53"/>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
       <c r="P20" s="18"/>
@@ -17688,28 +17778,28 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A21" s="53" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B21" s="53">
-        <v>2.9522508493098787E-2</v>
+        <v>0</v>
       </c>
       <c r="C21" s="53">
-        <v>-6.5382998365994035E-3</v>
+        <v>0</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E21" s="53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="53"/>
+        <v>58</v>
+      </c>
+      <c r="G21" s="53">
+        <v>0</v>
+      </c>
       <c r="H21" s="53"/>
-      <c r="I21" s="53">
-        <v>2.9522508493098787E-2</v>
-      </c>
+      <c r="I21" s="53"/>
       <c r="J21" s="53"/>
       <c r="P21" s="18"/>
       <c r="Q21" s="19"/>
@@ -17717,16 +17807,16 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A22" s="53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="53">
-        <v>11.741769456232131</v>
+        <v>0</v>
       </c>
       <c r="C22" s="53">
-        <v>1.4478162405317532</v>
+        <v>0</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="53">
         <v>2</v>
@@ -17763,7 +17853,7 @@
       <c r="J23" s="53"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R23" s="18"/>
     </row>
@@ -17894,7 +17984,7 @@
     <row r="48" spans="16:18" x14ac:dyDescent="0.4">
       <c r="P48" s="18"/>
       <c r="Q48" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R48" s="18"/>
     </row>
@@ -18386,7 +18476,7 @@
       <c r="O89" s="19"/>
       <c r="P89" s="81"/>
       <c r="Q89" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R89" s="83"/>
       <c r="S89" s="80"/>
@@ -18413,7 +18503,7 @@
       <c r="O90" s="19"/>
       <c r="P90" s="81"/>
       <c r="Q90" s="84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R90" s="81"/>
       <c r="U90" s="19"/>
@@ -18487,10 +18577,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C98E4FB-368A-4C5E-A56F-599B0C6D8A44}">
-  <dimension ref="A1:BB24"/>
+  <dimension ref="A1:BB37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22:AC22"/>
+      <selection activeCell="I37" sqref="I37:J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -18498,9 +18588,8 @@
     <col min="1" max="11" width="9.53515625" customWidth="1"/>
     <col min="12" max="12" width="14.61328125" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="14.61328125" customWidth="1"/>
-    <col min="15" max="15" width="23.61328125" customWidth="1"/>
-    <col min="16" max="16" width="1.84375" customWidth="1"/>
+    <col min="14" max="15" width="23.61328125" customWidth="1"/>
+    <col min="16" max="16" width="7.765625" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
     <col min="19" max="19" width="8.765625" customWidth="1"/>
@@ -18522,28 +18611,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>110</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>111</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>1</v>
@@ -18742,13 +18831,13 @@
         <v>0.96504087593346111</v>
       </c>
       <c r="H4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="J4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L4" t="s">
         <v>58</v>
@@ -18831,13 +18920,13 @@
         <v>0.96504087593346111</v>
       </c>
       <c r="H5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L5" t="s">
         <v>58</v>
@@ -18852,7 +18941,7 @@
         <v>55</v>
       </c>
       <c r="P5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q5" t="s">
         <v>65</v>
@@ -18920,13 +19009,13 @@
         <v>0.63581053785135866</v>
       </c>
       <c r="H6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" t="s">
         <v>58</v>
@@ -18941,7 +19030,7 @@
         <v>55</v>
       </c>
       <c r="P6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q6" t="s">
         <v>65</v>
@@ -19009,13 +19098,13 @@
         <v>0.7085546376937647</v>
       </c>
       <c r="H7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L7" t="s">
         <v>58</v>
@@ -19030,7 +19119,7 @@
         <v>55</v>
       </c>
       <c r="P7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q7" t="s">
         <v>65</v>
@@ -19098,13 +19187,13 @@
         <v>0.63581053785135866</v>
       </c>
       <c r="H8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L8" t="s">
         <v>58</v>
@@ -19119,7 +19208,7 @@
         <v>55</v>
       </c>
       <c r="P8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q8" t="s">
         <v>65</v>
@@ -19519,13 +19608,13 @@
         <v>0.96504087593346111</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L13" t="s">
         <v>58</v>
@@ -19540,7 +19629,7 @@
         <v>55</v>
       </c>
       <c r="P13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q13" t="s">
         <v>65</v>
@@ -19608,13 +19697,13 @@
         <v>0.96504087593346111</v>
       </c>
       <c r="H14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L14" t="s">
         <v>58</v>
@@ -19629,7 +19718,7 @@
         <v>55</v>
       </c>
       <c r="P14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Q14" t="s">
         <v>65</v>
@@ -19697,13 +19786,13 @@
         <v>1.0717045864387162</v>
       </c>
       <c r="H15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L15" t="s">
         <v>58</v>
@@ -19718,7 +19807,7 @@
         <v>55</v>
       </c>
       <c r="P15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q15" t="s">
         <v>65</v>
@@ -19786,13 +19875,13 @@
         <v>1.0717045864387162</v>
       </c>
       <c r="H16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L16" t="s">
         <v>58</v>
@@ -19807,7 +19896,7 @@
         <v>55</v>
       </c>
       <c r="P16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q16" t="s">
         <v>65</v>
@@ -19875,13 +19964,13 @@
         <v>0.7085546376937647</v>
       </c>
       <c r="H17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L17" t="s">
         <v>58</v>
@@ -19896,7 +19985,7 @@
         <v>55</v>
       </c>
       <c r="P17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q17" t="s">
         <v>65</v>
@@ -19964,13 +20053,13 @@
         <v>0.63581053785135866</v>
       </c>
       <c r="H18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L18" t="s">
         <v>58</v>
@@ -19985,7 +20074,7 @@
         <v>55</v>
       </c>
       <c r="P18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q18" t="s">
         <v>65</v>
@@ -20136,13 +20225,13 @@
         <v>0.75198237039542204</v>
       </c>
       <c r="H20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L20" t="s">
         <v>58</v>
@@ -20157,7 +20246,7 @@
         <v>55</v>
       </c>
       <c r="P20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q20" t="s">
         <v>65</v>
@@ -20366,21 +20455,1277 @@
       </c>
       <c r="AZ22" s="18"/>
       <c r="BA22" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB22" s="18"/>
     </row>
     <row r="23" spans="1:54" ht="17.149999999999999" x14ac:dyDescent="0.4">
+      <c r="A23" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B23">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C23" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D23" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E23">
+        <v>0.15</v>
+      </c>
+      <c r="F23">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G23">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H23" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" t="s">
+        <v>142</v>
+      </c>
+      <c r="J23" t="s">
+        <v>142</v>
+      </c>
+      <c r="L23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" t="s">
+        <v>55</v>
+      </c>
+      <c r="P23" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>65</v>
+      </c>
+      <c r="R23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23" t="s">
+        <v>71</v>
+      </c>
+      <c r="T23" t="s">
+        <v>70</v>
+      </c>
+      <c r="U23" t="s">
+        <v>74</v>
+      </c>
+      <c r="V23" t="s">
+        <v>68</v>
+      </c>
+      <c r="W23" t="s">
+        <v>73</v>
+      </c>
+      <c r="X23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>69</v>
+      </c>
       <c r="AZ23" s="18"/>
       <c r="BA23" s="84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BB23" s="18"/>
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A24" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B24">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C24" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D24" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E24">
+        <v>0.15</v>
+      </c>
+      <c r="F24">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G24">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" t="s">
+        <v>144</v>
+      </c>
+      <c r="L24" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" t="s">
+        <v>59</v>
+      </c>
+      <c r="N24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>65</v>
+      </c>
+      <c r="R24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24" t="s">
+        <v>71</v>
+      </c>
+      <c r="T24" t="s">
+        <v>70</v>
+      </c>
+      <c r="U24" t="s">
+        <v>74</v>
+      </c>
+      <c r="V24" t="s">
+        <v>68</v>
+      </c>
+      <c r="W24" t="s">
+        <v>73</v>
+      </c>
+      <c r="X24" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>69</v>
+      </c>
       <c r="AZ24" s="18"/>
       <c r="BA24" s="18"/>
       <c r="BB24" s="18"/>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B25">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C25" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D25" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E25">
+        <v>0.15</v>
+      </c>
+      <c r="F25">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G25">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H25" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" t="s">
+        <v>146</v>
+      </c>
+      <c r="J25" t="s">
+        <v>146</v>
+      </c>
+      <c r="L25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" t="s">
+        <v>55</v>
+      </c>
+      <c r="P25" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>65</v>
+      </c>
+      <c r="R25" t="s">
+        <v>64</v>
+      </c>
+      <c r="S25" t="s">
+        <v>71</v>
+      </c>
+      <c r="T25" t="s">
+        <v>70</v>
+      </c>
+      <c r="U25" t="s">
+        <v>74</v>
+      </c>
+      <c r="V25" t="s">
+        <v>68</v>
+      </c>
+      <c r="W25" t="s">
+        <v>73</v>
+      </c>
+      <c r="X25" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A26" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B26">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C26" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D26" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E26">
+        <v>0.15</v>
+      </c>
+      <c r="F26">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G26">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H26" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J26" t="s">
+        <v>148</v>
+      </c>
+      <c r="L26" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" t="s">
+        <v>60</v>
+      </c>
+      <c r="O26" t="s">
+        <v>55</v>
+      </c>
+      <c r="P26" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>65</v>
+      </c>
+      <c r="R26" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26" t="s">
+        <v>71</v>
+      </c>
+      <c r="T26" t="s">
+        <v>70</v>
+      </c>
+      <c r="U26" t="s">
+        <v>74</v>
+      </c>
+      <c r="V26" t="s">
+        <v>68</v>
+      </c>
+      <c r="W26" t="s">
+        <v>73</v>
+      </c>
+      <c r="X26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A27" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B27">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C27" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D27" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E27">
+        <v>0.15</v>
+      </c>
+      <c r="F27">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G27">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" t="s">
+        <v>150</v>
+      </c>
+      <c r="J27" t="s">
+        <v>150</v>
+      </c>
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" t="s">
+        <v>59</v>
+      </c>
+      <c r="N27" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" t="s">
+        <v>55</v>
+      </c>
+      <c r="P27" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>65</v>
+      </c>
+      <c r="R27" t="s">
+        <v>64</v>
+      </c>
+      <c r="S27" t="s">
+        <v>71</v>
+      </c>
+      <c r="T27" t="s">
+        <v>70</v>
+      </c>
+      <c r="U27" t="s">
+        <v>74</v>
+      </c>
+      <c r="V27" t="s">
+        <v>68</v>
+      </c>
+      <c r="W27" t="s">
+        <v>73</v>
+      </c>
+      <c r="X27" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A28" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B28">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C28" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D28" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E28">
+        <v>0.15</v>
+      </c>
+      <c r="F28">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G28">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H28" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" t="s">
+        <v>152</v>
+      </c>
+      <c r="J28" t="s">
+        <v>152</v>
+      </c>
+      <c r="L28" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
+      </c>
+      <c r="O28" t="s">
+        <v>55</v>
+      </c>
+      <c r="P28" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>65</v>
+      </c>
+      <c r="R28" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T28" t="s">
+        <v>70</v>
+      </c>
+      <c r="U28" t="s">
+        <v>74</v>
+      </c>
+      <c r="V28" t="s">
+        <v>68</v>
+      </c>
+      <c r="W28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X28" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A29" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B29">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C29" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D29" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E29">
+        <v>0.15</v>
+      </c>
+      <c r="F29">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G29">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29" t="s">
+        <v>154</v>
+      </c>
+      <c r="J29" t="s">
+        <v>154</v>
+      </c>
+      <c r="L29" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N29" t="s">
+        <v>60</v>
+      </c>
+      <c r="O29" t="s">
+        <v>55</v>
+      </c>
+      <c r="P29" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>65</v>
+      </c>
+      <c r="R29" t="s">
+        <v>64</v>
+      </c>
+      <c r="S29" t="s">
+        <v>71</v>
+      </c>
+      <c r="T29" t="s">
+        <v>70</v>
+      </c>
+      <c r="U29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V29" t="s">
+        <v>68</v>
+      </c>
+      <c r="W29" t="s">
+        <v>73</v>
+      </c>
+      <c r="X29" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A30" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B30">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C30" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D30" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E30">
+        <v>0.15</v>
+      </c>
+      <c r="F30">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G30">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I30" t="s">
+        <v>156</v>
+      </c>
+      <c r="J30" t="s">
+        <v>156</v>
+      </c>
+      <c r="L30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" t="s">
+        <v>60</v>
+      </c>
+      <c r="O30" t="s">
+        <v>55</v>
+      </c>
+      <c r="P30" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>65</v>
+      </c>
+      <c r="R30" t="s">
+        <v>64</v>
+      </c>
+      <c r="S30" t="s">
+        <v>71</v>
+      </c>
+      <c r="T30" t="s">
+        <v>70</v>
+      </c>
+      <c r="U30" t="s">
+        <v>74</v>
+      </c>
+      <c r="V30" t="s">
+        <v>68</v>
+      </c>
+      <c r="W30" t="s">
+        <v>73</v>
+      </c>
+      <c r="X30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A31" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B31">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C31" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D31" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E31">
+        <v>0.15</v>
+      </c>
+      <c r="F31">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G31">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H31" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" t="s">
+        <v>158</v>
+      </c>
+      <c r="J31" t="s">
+        <v>158</v>
+      </c>
+      <c r="L31" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" t="s">
+        <v>60</v>
+      </c>
+      <c r="O31" t="s">
+        <v>55</v>
+      </c>
+      <c r="P31" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>65</v>
+      </c>
+      <c r="R31" t="s">
+        <v>64</v>
+      </c>
+      <c r="S31" t="s">
+        <v>71</v>
+      </c>
+      <c r="T31" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" t="s">
+        <v>74</v>
+      </c>
+      <c r="V31" t="s">
+        <v>68</v>
+      </c>
+      <c r="W31" t="s">
+        <v>73</v>
+      </c>
+      <c r="X31" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A32" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B32">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C32" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D32" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E32">
+        <v>0.15</v>
+      </c>
+      <c r="F32">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G32">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H32" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" t="s">
+        <v>160</v>
+      </c>
+      <c r="J32" t="s">
+        <v>160</v>
+      </c>
+      <c r="L32" t="s">
+        <v>58</v>
+      </c>
+      <c r="M32" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" t="s">
+        <v>60</v>
+      </c>
+      <c r="O32" t="s">
+        <v>55</v>
+      </c>
+      <c r="P32" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>65</v>
+      </c>
+      <c r="R32" t="s">
+        <v>64</v>
+      </c>
+      <c r="S32" t="s">
+        <v>71</v>
+      </c>
+      <c r="T32" t="s">
+        <v>70</v>
+      </c>
+      <c r="U32" t="s">
+        <v>74</v>
+      </c>
+      <c r="V32" t="s">
+        <v>68</v>
+      </c>
+      <c r="W32" t="s">
+        <v>73</v>
+      </c>
+      <c r="X32" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A33" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B33">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C33" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D33" s="45">
+        <v>0.44</v>
+      </c>
+      <c r="E33">
+        <v>0.25666371050525516</v>
+      </c>
+      <c r="F33">
+        <v>0.55837716542820592</v>
+      </c>
+      <c r="G33">
+        <v>1.0717045864387162</v>
+      </c>
+      <c r="H33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I33" t="s">
+        <v>162</v>
+      </c>
+      <c r="J33" t="s">
+        <v>162</v>
+      </c>
+      <c r="L33" t="s">
+        <v>58</v>
+      </c>
+      <c r="M33" t="s">
+        <v>59</v>
+      </c>
+      <c r="N33" t="s">
+        <v>60</v>
+      </c>
+      <c r="O33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P33" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R33" t="s">
+        <v>64</v>
+      </c>
+      <c r="S33" t="s">
+        <v>71</v>
+      </c>
+      <c r="T33" t="s">
+        <v>70</v>
+      </c>
+      <c r="U33" t="s">
+        <v>74</v>
+      </c>
+      <c r="V33" t="s">
+        <v>68</v>
+      </c>
+      <c r="W33" t="s">
+        <v>73</v>
+      </c>
+      <c r="X33" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A34" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B34">
+        <v>0.81504087593346108</v>
+      </c>
+      <c r="C34" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D34" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E34">
+        <v>0.15</v>
+      </c>
+      <c r="F34">
+        <v>0.66504087593346106</v>
+      </c>
+      <c r="G34">
+        <v>0.96504087593346111</v>
+      </c>
+      <c r="H34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" t="s">
+        <v>164</v>
+      </c>
+      <c r="J34" t="s">
+        <v>164</v>
+      </c>
+      <c r="L34" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" t="s">
+        <v>59</v>
+      </c>
+      <c r="N34" t="s">
+        <v>60</v>
+      </c>
+      <c r="O34" t="s">
+        <v>55</v>
+      </c>
+      <c r="P34" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>65</v>
+      </c>
+      <c r="R34" t="s">
+        <v>64</v>
+      </c>
+      <c r="S34" t="s">
+        <v>71</v>
+      </c>
+      <c r="T34" t="s">
+        <v>70</v>
+      </c>
+      <c r="U34" t="s">
+        <v>74</v>
+      </c>
+      <c r="V34" t="s">
+        <v>68</v>
+      </c>
+      <c r="W34" t="s">
+        <v>73</v>
+      </c>
+      <c r="X34" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A35" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B35">
+        <v>0.74947496215707643</v>
+      </c>
+      <c r="C35" s="45">
+        <v>0.44</v>
+      </c>
+      <c r="D35" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E35">
+        <v>0.15</v>
+      </c>
+      <c r="F35">
+        <v>0.59947496215707641</v>
+      </c>
+      <c r="G35">
+        <v>0.89947496215707645</v>
+      </c>
+      <c r="H35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" t="s">
+        <v>166</v>
+      </c>
+      <c r="J35" t="s">
+        <v>166</v>
+      </c>
+      <c r="L35" t="s">
+        <v>58</v>
+      </c>
+      <c r="M35" t="s">
+        <v>59</v>
+      </c>
+      <c r="N35" t="s">
+        <v>55</v>
+      </c>
+      <c r="O35" t="s">
+        <v>165</v>
+      </c>
+      <c r="P35" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>64</v>
+      </c>
+      <c r="R35" t="s">
+        <v>71</v>
+      </c>
+      <c r="S35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A36" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B36">
+        <v>0.48581053785135864</v>
+      </c>
+      <c r="C36" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D36" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E36">
+        <v>0.15</v>
+      </c>
+      <c r="F36">
+        <v>0.33581053785135861</v>
+      </c>
+      <c r="G36">
+        <v>0.63581053785135866</v>
+      </c>
+      <c r="H36" t="s">
+        <v>117</v>
+      </c>
+      <c r="I36" t="s">
+        <v>168</v>
+      </c>
+      <c r="J36" t="s">
+        <v>168</v>
+      </c>
+      <c r="L36" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" t="s">
+        <v>59</v>
+      </c>
+      <c r="N36" t="s">
+        <v>60</v>
+      </c>
+      <c r="O36" t="s">
+        <v>55</v>
+      </c>
+      <c r="P36" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>65</v>
+      </c>
+      <c r="R36" t="s">
+        <v>64</v>
+      </c>
+      <c r="S36" t="s">
+        <v>71</v>
+      </c>
+      <c r="T36" t="s">
+        <v>70</v>
+      </c>
+      <c r="U36" t="s">
+        <v>74</v>
+      </c>
+      <c r="V36" t="s">
+        <v>68</v>
+      </c>
+      <c r="W36" t="s">
+        <v>73</v>
+      </c>
+      <c r="X36" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A37" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B37">
+        <v>0.55855463769376468</v>
+      </c>
+      <c r="C37" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="D37" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E37">
+        <v>0.15</v>
+      </c>
+      <c r="F37">
+        <v>0.40855463769376466</v>
+      </c>
+      <c r="G37">
+        <v>0.7085546376937647</v>
+      </c>
+      <c r="H37" t="s">
+        <v>117</v>
+      </c>
+      <c r="I37" t="s">
+        <v>171</v>
+      </c>
+      <c r="J37" t="s">
+        <v>171</v>
+      </c>
+      <c r="L37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M37" t="s">
+        <v>59</v>
+      </c>
+      <c r="N37" t="s">
+        <v>60</v>
+      </c>
+      <c r="O37" t="s">
+        <v>55</v>
+      </c>
+      <c r="P37" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>65</v>
+      </c>
+      <c r="R37" t="s">
+        <v>64</v>
+      </c>
+      <c r="S37" t="s">
+        <v>71</v>
+      </c>
+      <c r="T37" t="s">
+        <v>70</v>
+      </c>
+      <c r="U37" t="s">
+        <v>74</v>
+      </c>
+      <c r="V37" t="s">
+        <v>68</v>
+      </c>
+      <c r="W37" t="s">
+        <v>73</v>
+      </c>
+      <c r="X37" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20390,19 +21735,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8347BB22-A19A-404F-8113-FCDA6D177D04}">
-  <dimension ref="A1:BB24"/>
+  <dimension ref="A1:BB37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22:AC22"/>
+      <selection activeCell="A37" sqref="A37:K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="11" width="9.53515625" customWidth="1"/>
     <col min="12" max="12" width="13.61328125" customWidth="1"/>
-    <col min="13" max="14" width="14.61328125" customWidth="1"/>
-    <col min="15" max="15" width="23.61328125" customWidth="1"/>
-    <col min="16" max="16" width="1.84375" customWidth="1"/>
+    <col min="13" max="13" width="14.61328125" customWidth="1"/>
+    <col min="14" max="15" width="23.61328125" customWidth="1"/>
+    <col min="16" max="16" width="7.765625" customWidth="1"/>
     <col min="17" max="17" width="14.61328125" customWidth="1"/>
     <col min="18" max="18" width="15.61328125" customWidth="1"/>
     <col min="19" max="19" width="8.765625" customWidth="1"/>
@@ -20425,28 +21770,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>110</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>111</v>
       </c>
       <c r="H1" s="27" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>1</v>
@@ -20643,7 +21988,7 @@
         <v>1.3278795103679406</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L4" t="s">
         <v>58</v>
@@ -20658,7 +22003,7 @@
         <v>55</v>
       </c>
       <c r="P4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q4" t="s">
         <v>65</v>
@@ -20726,7 +22071,7 @@
         <v>1.3278795103679406</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L5" t="s">
         <v>58</v>
@@ -20741,7 +22086,7 @@
         <v>55</v>
       </c>
       <c r="P5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q5" t="s">
         <v>65</v>
@@ -20809,7 +22154,7 @@
         <v>0.54423539039701896</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L6" t="s">
         <v>58</v>
@@ -20824,7 +22169,7 @@
         <v>55</v>
       </c>
       <c r="P6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q6" t="s">
         <v>65</v>
@@ -20892,7 +22237,7 @@
         <v>0.85434105290898843</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L7" t="s">
         <v>58</v>
@@ -20907,7 +22252,7 @@
         <v>55</v>
       </c>
       <c r="P7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Q7" t="s">
         <v>65</v>
@@ -20975,7 +22320,7 @@
         <v>0.54423539039701896</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L8" t="s">
         <v>58</v>
@@ -20990,7 +22335,7 @@
         <v>55</v>
       </c>
       <c r="P8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q8" t="s">
         <v>65</v>
@@ -21390,7 +22735,7 @@
         <v>1.3278795103679406</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L13" t="s">
         <v>58</v>
@@ -21405,7 +22750,7 @@
         <v>55</v>
       </c>
       <c r="P13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q13" t="s">
         <v>65</v>
@@ -21473,7 +22818,7 @@
         <v>1.3278795103679406</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L14" t="s">
         <v>58</v>
@@ -21488,7 +22833,7 @@
         <v>55</v>
       </c>
       <c r="P14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q14" t="s">
         <v>65</v>
@@ -21556,7 +22901,7 @@
         <v>1.3932851270715454</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L15" t="s">
         <v>58</v>
@@ -21571,7 +22916,7 @@
         <v>55</v>
       </c>
       <c r="P15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q15" t="s">
         <v>65</v>
@@ -21639,7 +22984,7 @@
         <v>1.3932851270715454</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L16" t="s">
         <v>58</v>
@@ -21654,7 +22999,7 @@
         <v>55</v>
       </c>
       <c r="P16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q16" t="s">
         <v>65</v>
@@ -21722,7 +23067,7 @@
         <v>0.85434105290898843</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L17" t="s">
         <v>58</v>
@@ -21737,7 +23082,7 @@
         <v>55</v>
       </c>
       <c r="P17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q17" t="s">
         <v>65</v>
@@ -21805,7 +23150,7 @@
         <v>0.54423539039701896</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L18" t="s">
         <v>58</v>
@@ -21820,7 +23165,7 @@
         <v>55</v>
       </c>
       <c r="P18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q18" t="s">
         <v>65</v>
@@ -21971,7 +23316,7 @@
         <v>0.60254795978646492</v>
       </c>
       <c r="I20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L20" t="s">
         <v>58</v>
@@ -21986,7 +23331,7 @@
         <v>55</v>
       </c>
       <c r="P20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q20" t="s">
         <v>65</v>
@@ -22195,21 +23540,1187 @@
       </c>
       <c r="AZ22" s="18"/>
       <c r="BA22" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BB22" s="18"/>
     </row>
     <row r="23" spans="1:54" ht="17.149999999999999" x14ac:dyDescent="0.4">
+      <c r="A23" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B23">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C23" s="45">
+        <v>0</v>
+      </c>
+      <c r="D23" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E23">
+        <v>0.21</v>
+      </c>
+      <c r="F23">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G23">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I23" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" t="s">
+        <v>59</v>
+      </c>
+      <c r="N23" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" t="s">
+        <v>55</v>
+      </c>
+      <c r="P23" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>65</v>
+      </c>
+      <c r="R23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23" t="s">
+        <v>71</v>
+      </c>
+      <c r="T23" t="s">
+        <v>70</v>
+      </c>
+      <c r="U23" t="s">
+        <v>74</v>
+      </c>
+      <c r="V23" t="s">
+        <v>68</v>
+      </c>
+      <c r="W23" t="s">
+        <v>73</v>
+      </c>
+      <c r="X23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>69</v>
+      </c>
       <c r="AZ23" s="18"/>
       <c r="BA23" s="84" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BB23" s="18"/>
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A24" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B24">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C24" s="45">
+        <v>0</v>
+      </c>
+      <c r="D24" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E24">
+        <v>0.21</v>
+      </c>
+      <c r="F24">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G24">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" t="s">
+        <v>58</v>
+      </c>
+      <c r="M24" t="s">
+        <v>59</v>
+      </c>
+      <c r="N24" t="s">
+        <v>60</v>
+      </c>
+      <c r="O24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>65</v>
+      </c>
+      <c r="R24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24" t="s">
+        <v>71</v>
+      </c>
+      <c r="T24" t="s">
+        <v>70</v>
+      </c>
+      <c r="U24" t="s">
+        <v>74</v>
+      </c>
+      <c r="V24" t="s">
+        <v>68</v>
+      </c>
+      <c r="W24" t="s">
+        <v>73</v>
+      </c>
+      <c r="X24" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>69</v>
+      </c>
       <c r="AZ24" s="18"/>
       <c r="BA24" s="18"/>
       <c r="BB24" s="18"/>
+    </row>
+    <row r="25" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A25" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B25">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C25" s="45">
+        <v>0</v>
+      </c>
+      <c r="D25" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E25">
+        <v>0.21</v>
+      </c>
+      <c r="F25">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G25">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I25" t="s">
+        <v>117</v>
+      </c>
+      <c r="L25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" t="s">
+        <v>55</v>
+      </c>
+      <c r="P25" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>65</v>
+      </c>
+      <c r="R25" t="s">
+        <v>64</v>
+      </c>
+      <c r="S25" t="s">
+        <v>71</v>
+      </c>
+      <c r="T25" t="s">
+        <v>70</v>
+      </c>
+      <c r="U25" t="s">
+        <v>74</v>
+      </c>
+      <c r="V25" t="s">
+        <v>68</v>
+      </c>
+      <c r="W25" t="s">
+        <v>73</v>
+      </c>
+      <c r="X25" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A26" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B26">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C26" s="45">
+        <v>0</v>
+      </c>
+      <c r="D26" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E26">
+        <v>0.21</v>
+      </c>
+      <c r="F26">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G26">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I26" t="s">
+        <v>117</v>
+      </c>
+      <c r="L26" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N26" t="s">
+        <v>60</v>
+      </c>
+      <c r="O26" t="s">
+        <v>55</v>
+      </c>
+      <c r="P26" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>65</v>
+      </c>
+      <c r="R26" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26" t="s">
+        <v>71</v>
+      </c>
+      <c r="T26" t="s">
+        <v>70</v>
+      </c>
+      <c r="U26" t="s">
+        <v>74</v>
+      </c>
+      <c r="V26" t="s">
+        <v>68</v>
+      </c>
+      <c r="W26" t="s">
+        <v>73</v>
+      </c>
+      <c r="X26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A27" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B27">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C27" s="45">
+        <v>0</v>
+      </c>
+      <c r="D27" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E27">
+        <v>0.21</v>
+      </c>
+      <c r="F27">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G27">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I27" t="s">
+        <v>117</v>
+      </c>
+      <c r="L27" t="s">
+        <v>58</v>
+      </c>
+      <c r="M27" t="s">
+        <v>59</v>
+      </c>
+      <c r="N27" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" t="s">
+        <v>55</v>
+      </c>
+      <c r="P27" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>65</v>
+      </c>
+      <c r="R27" t="s">
+        <v>64</v>
+      </c>
+      <c r="S27" t="s">
+        <v>71</v>
+      </c>
+      <c r="T27" t="s">
+        <v>70</v>
+      </c>
+      <c r="U27" t="s">
+        <v>74</v>
+      </c>
+      <c r="V27" t="s">
+        <v>68</v>
+      </c>
+      <c r="W27" t="s">
+        <v>73</v>
+      </c>
+      <c r="X27" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A28" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B28">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C28" s="45">
+        <v>0</v>
+      </c>
+      <c r="D28" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E28">
+        <v>0.21</v>
+      </c>
+      <c r="F28">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G28">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I28" t="s">
+        <v>117</v>
+      </c>
+      <c r="L28" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" t="s">
+        <v>59</v>
+      </c>
+      <c r="N28" t="s">
+        <v>60</v>
+      </c>
+      <c r="O28" t="s">
+        <v>55</v>
+      </c>
+      <c r="P28" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>65</v>
+      </c>
+      <c r="R28" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28" t="s">
+        <v>71</v>
+      </c>
+      <c r="T28" t="s">
+        <v>70</v>
+      </c>
+      <c r="U28" t="s">
+        <v>74</v>
+      </c>
+      <c r="V28" t="s">
+        <v>68</v>
+      </c>
+      <c r="W28" t="s">
+        <v>73</v>
+      </c>
+      <c r="X28" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A29" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B29">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C29" s="45">
+        <v>0</v>
+      </c>
+      <c r="D29" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E29">
+        <v>0.21</v>
+      </c>
+      <c r="F29">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G29">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I29" t="s">
+        <v>117</v>
+      </c>
+      <c r="L29" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" t="s">
+        <v>59</v>
+      </c>
+      <c r="N29" t="s">
+        <v>60</v>
+      </c>
+      <c r="O29" t="s">
+        <v>55</v>
+      </c>
+      <c r="P29" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>65</v>
+      </c>
+      <c r="R29" t="s">
+        <v>64</v>
+      </c>
+      <c r="S29" t="s">
+        <v>71</v>
+      </c>
+      <c r="T29" t="s">
+        <v>70</v>
+      </c>
+      <c r="U29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V29" t="s">
+        <v>68</v>
+      </c>
+      <c r="W29" t="s">
+        <v>73</v>
+      </c>
+      <c r="X29" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A30" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B30">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C30" s="45">
+        <v>0</v>
+      </c>
+      <c r="D30" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E30">
+        <v>0.21</v>
+      </c>
+      <c r="F30">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G30">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I30" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" t="s">
+        <v>58</v>
+      </c>
+      <c r="M30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" t="s">
+        <v>60</v>
+      </c>
+      <c r="O30" t="s">
+        <v>55</v>
+      </c>
+      <c r="P30" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>65</v>
+      </c>
+      <c r="R30" t="s">
+        <v>64</v>
+      </c>
+      <c r="S30" t="s">
+        <v>71</v>
+      </c>
+      <c r="T30" t="s">
+        <v>70</v>
+      </c>
+      <c r="U30" t="s">
+        <v>74</v>
+      </c>
+      <c r="V30" t="s">
+        <v>68</v>
+      </c>
+      <c r="W30" t="s">
+        <v>73</v>
+      </c>
+      <c r="X30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A31" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B31">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C31" s="45">
+        <v>0</v>
+      </c>
+      <c r="D31" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E31">
+        <v>0.21</v>
+      </c>
+      <c r="F31">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G31">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I31" t="s">
+        <v>117</v>
+      </c>
+      <c r="L31" t="s">
+        <v>58</v>
+      </c>
+      <c r="M31" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" t="s">
+        <v>60</v>
+      </c>
+      <c r="O31" t="s">
+        <v>55</v>
+      </c>
+      <c r="P31" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>65</v>
+      </c>
+      <c r="R31" t="s">
+        <v>64</v>
+      </c>
+      <c r="S31" t="s">
+        <v>71</v>
+      </c>
+      <c r="T31" t="s">
+        <v>70</v>
+      </c>
+      <c r="U31" t="s">
+        <v>74</v>
+      </c>
+      <c r="V31" t="s">
+        <v>68</v>
+      </c>
+      <c r="W31" t="s">
+        <v>73</v>
+      </c>
+      <c r="X31" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:54" x14ac:dyDescent="0.4">
+      <c r="A32" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B32">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C32" s="45">
+        <v>0</v>
+      </c>
+      <c r="D32" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E32">
+        <v>0.21</v>
+      </c>
+      <c r="F32">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G32">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I32" t="s">
+        <v>117</v>
+      </c>
+      <c r="L32" t="s">
+        <v>58</v>
+      </c>
+      <c r="M32" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" t="s">
+        <v>60</v>
+      </c>
+      <c r="O32" t="s">
+        <v>55</v>
+      </c>
+      <c r="P32" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>65</v>
+      </c>
+      <c r="R32" t="s">
+        <v>64</v>
+      </c>
+      <c r="S32" t="s">
+        <v>71</v>
+      </c>
+      <c r="T32" t="s">
+        <v>70</v>
+      </c>
+      <c r="U32" t="s">
+        <v>74</v>
+      </c>
+      <c r="V32" t="s">
+        <v>68</v>
+      </c>
+      <c r="W32" t="s">
+        <v>73</v>
+      </c>
+      <c r="X32" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A33" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B33">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C33" s="45">
+        <v>0</v>
+      </c>
+      <c r="D33" s="45">
+        <v>0.32</v>
+      </c>
+      <c r="E33">
+        <v>0.30540561670360467</v>
+      </c>
+      <c r="F33">
+        <v>0.78247389366433595</v>
+      </c>
+      <c r="G33">
+        <v>1.3932851270715454</v>
+      </c>
+      <c r="I33" t="s">
+        <v>117</v>
+      </c>
+      <c r="L33" t="s">
+        <v>58</v>
+      </c>
+      <c r="M33" t="s">
+        <v>59</v>
+      </c>
+      <c r="N33" t="s">
+        <v>60</v>
+      </c>
+      <c r="O33" t="s">
+        <v>55</v>
+      </c>
+      <c r="P33" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>65</v>
+      </c>
+      <c r="R33" t="s">
+        <v>64</v>
+      </c>
+      <c r="S33" t="s">
+        <v>71</v>
+      </c>
+      <c r="T33" t="s">
+        <v>70</v>
+      </c>
+      <c r="U33" t="s">
+        <v>74</v>
+      </c>
+      <c r="V33" t="s">
+        <v>68</v>
+      </c>
+      <c r="W33" t="s">
+        <v>73</v>
+      </c>
+      <c r="X33" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A34" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B34">
+        <v>1.0878795103679406</v>
+      </c>
+      <c r="C34" s="45">
+        <v>0</v>
+      </c>
+      <c r="D34" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E34">
+        <v>0.21</v>
+      </c>
+      <c r="F34">
+        <v>0.87787951036794065</v>
+      </c>
+      <c r="G34">
+        <v>1.2978795103679406</v>
+      </c>
+      <c r="I34" t="s">
+        <v>117</v>
+      </c>
+      <c r="L34" t="s">
+        <v>58</v>
+      </c>
+      <c r="M34" t="s">
+        <v>59</v>
+      </c>
+      <c r="N34" t="s">
+        <v>60</v>
+      </c>
+      <c r="O34" t="s">
+        <v>55</v>
+      </c>
+      <c r="P34" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>65</v>
+      </c>
+      <c r="R34" t="s">
+        <v>64</v>
+      </c>
+      <c r="S34" t="s">
+        <v>71</v>
+      </c>
+      <c r="T34" t="s">
+        <v>70</v>
+      </c>
+      <c r="U34" t="s">
+        <v>74</v>
+      </c>
+      <c r="V34" t="s">
+        <v>68</v>
+      </c>
+      <c r="W34" t="s">
+        <v>73</v>
+      </c>
+      <c r="X34" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A35" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B35">
+        <v>0.58037448000514547</v>
+      </c>
+      <c r="C35" s="45">
+        <v>0</v>
+      </c>
+      <c r="D35" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E35">
+        <v>0.21</v>
+      </c>
+      <c r="F35">
+        <v>0.3703744800051455</v>
+      </c>
+      <c r="G35">
+        <v>0.79037448000514543</v>
+      </c>
+      <c r="I35" t="s">
+        <v>117</v>
+      </c>
+      <c r="L35" t="s">
+        <v>58</v>
+      </c>
+      <c r="M35" t="s">
+        <v>59</v>
+      </c>
+      <c r="N35" t="s">
+        <v>55</v>
+      </c>
+      <c r="O35" t="s">
+        <v>166</v>
+      </c>
+      <c r="P35" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>64</v>
+      </c>
+      <c r="R35" t="s">
+        <v>71</v>
+      </c>
+      <c r="S35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A36" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B36">
+        <v>0.30423539039701897</v>
+      </c>
+      <c r="C36" s="45">
+        <v>0</v>
+      </c>
+      <c r="D36" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E36">
+        <v>0.21</v>
+      </c>
+      <c r="F36">
+        <v>9.4235390397018975E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.51423539039701893</v>
+      </c>
+      <c r="I36" t="s">
+        <v>117</v>
+      </c>
+      <c r="L36" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" t="s">
+        <v>59</v>
+      </c>
+      <c r="N36" t="s">
+        <v>60</v>
+      </c>
+      <c r="O36" t="s">
+        <v>55</v>
+      </c>
+      <c r="P36" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>65</v>
+      </c>
+      <c r="R36" t="s">
+        <v>64</v>
+      </c>
+      <c r="S36" t="s">
+        <v>71</v>
+      </c>
+      <c r="T36" t="s">
+        <v>70</v>
+      </c>
+      <c r="U36" t="s">
+        <v>74</v>
+      </c>
+      <c r="V36" t="s">
+        <v>68</v>
+      </c>
+      <c r="W36" t="s">
+        <v>73</v>
+      </c>
+      <c r="X36" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.4">
+      <c r="A37" s="1">
+        <v>46009</v>
+      </c>
+      <c r="B37">
+        <v>0.61434105290898844</v>
+      </c>
+      <c r="C37" s="45">
+        <v>0</v>
+      </c>
+      <c r="D37" s="45">
+        <v>0.88</v>
+      </c>
+      <c r="E37">
+        <v>0.21</v>
+      </c>
+      <c r="F37">
+        <v>0.40434105290898847</v>
+      </c>
+      <c r="G37">
+        <v>0.8243410529089884</v>
+      </c>
+      <c r="I37" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M37" t="s">
+        <v>59</v>
+      </c>
+      <c r="N37" t="s">
+        <v>60</v>
+      </c>
+      <c r="O37" t="s">
+        <v>55</v>
+      </c>
+      <c r="P37" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>65</v>
+      </c>
+      <c r="R37" t="s">
+        <v>64</v>
+      </c>
+      <c r="S37" t="s">
+        <v>71</v>
+      </c>
+      <c r="T37" t="s">
+        <v>70</v>
+      </c>
+      <c r="U37" t="s">
+        <v>74</v>
+      </c>
+      <c r="V37" t="s">
+        <v>68</v>
+      </c>
+      <c r="W37" t="s">
+        <v>73</v>
+      </c>
+      <c r="X37" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>